<commit_message>
added FETs and related circuitry for the motor drive, current sense
</commit_message>
<xml_diff>
--- a/eagle/bom.xlsx
+++ b/eagle/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\prj\qc\eagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE70CCE-0B35-413E-B11D-E3175D8C452A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D518B1-DFB7-4222-8486-F777EAAD5928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="507" windowWidth="25786" windowHeight="13986" xr2:uid="{7FFDE957-DDFA-40C3-B4B1-FC23B9487616}"/>
+    <workbookView xWindow="-93" yWindow="507" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{7FFDE957-DDFA-40C3-B4B1-FC23B9487616}"/>
   </bookViews>
   <sheets>
     <sheet name="ESC" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>MFG NUM</t>
   </si>
@@ -132,6 +132,12 @@
   <si>
     <t>Power 2-pin connector on board for 3.3V
 I2C bus usage as well</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/BLACK-DECKER-4-Slice-Convection-TO1750SB/dp/B071WXD3HX/ref=sr_1_15?keywords=toaster+oven&amp;qid=1578617961&amp;sr=8-15</t>
+  </si>
+  <si>
+    <t>toaster oven</t>
   </si>
 </sst>
 </file>
@@ -525,9 +531,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA596EF-40FD-4069-B258-04479C4B0B2E}">
   <dimension ref="A2:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -852,10 +858,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3555E04D-A003-41C2-8A9A-B1D0F27D6347}">
-  <dimension ref="A4:B4"/>
+  <dimension ref="A4:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -871,6 +877,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added most of the components to the schematic. Left to add connectors for SPI port for micro and power connectors
</commit_message>
<xml_diff>
--- a/eagle/bom.xlsx
+++ b/eagle/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\prj\qc\eagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D518B1-DFB7-4222-8486-F777EAAD5928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5A3C06-BED3-479D-8B8A-B6C28AB462C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="507" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{7FFDE957-DDFA-40C3-B4B1-FC23B9487616}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7FFDE957-DDFA-40C3-B4B1-FC23B9487616}"/>
   </bookViews>
   <sheets>
     <sheet name="ESC" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>MFG NUM</t>
   </si>
@@ -138,6 +138,87 @@
   </si>
   <si>
     <t>toaster oven</t>
+  </si>
+  <si>
+    <t>576-1910-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIC5319-3.3YD5-TR </t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/MIC5319-3-3YD5-TR/576-1910-1-ND/1799517</t>
+  </si>
+  <si>
+    <t>LDO for 5V to 3.3V</t>
+  </si>
+  <si>
+    <t>497-6447-1-ND</t>
+  </si>
+  <si>
+    <t>LD1117S50TR</t>
+  </si>
+  <si>
+    <t>12V to 5V regulator</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stmicroelectronics/LD1117S50TR/497-6447-1-ND/1865475</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stmicroelectronics/STLINK-V3SET/497-18216-ND/9636028</t>
+  </si>
+  <si>
+    <t>497-18216-ND</t>
+  </si>
+  <si>
+    <t>STLINK-V3SET</t>
+  </si>
+  <si>
+    <t>SAM13165CT-ND</t>
+  </si>
+  <si>
+    <t>FTSH-105-01-L-DV-K-TR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=SAM13165CT-ND</t>
+  </si>
+  <si>
+    <t>ARM10 connector</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/omron-electronics-inc-emc-div/B3F-1020/SW402-ND/44059</t>
+  </si>
+  <si>
+    <t>SW402-ND</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 24V</t>
+  </si>
+  <si>
+    <t>B3F-1020</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stmicroelectronics/STPS2L30A/497-3759-1-ND/691929</t>
+  </si>
+  <si>
+    <t>497-3759-1-ND</t>
+  </si>
+  <si>
+    <t>STPS2L30A</t>
+  </si>
+  <si>
+    <t>Diode Schottky 30V 2A Surface Mount SMA</t>
+  </si>
+  <si>
+    <t>PCE3948CT-ND</t>
+  </si>
+  <si>
+    <t>EEE-1VA100WR</t>
+  </si>
+  <si>
+    <t>10µF 35V Aluminum Electrolytic Capacitors Radial, Can - SMD  1000 Hrs @ 85°C</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/EEE-1VA100WR/PCE3948CT-ND/766324</t>
   </si>
 </sst>
 </file>
@@ -529,32 +610,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA596EF-40FD-4069-B258-04479C4B0B2E}">
-  <dimension ref="A2:G33"/>
+  <dimension ref="A2:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.64453125" customWidth="1"/>
-    <col min="2" max="2" width="15.64453125" customWidth="1"/>
-    <col min="3" max="3" width="8.9375" style="5"/>
-    <col min="5" max="5" width="8.9375" style="5"/>
-    <col min="6" max="6" width="60.64453125" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9" style="5"/>
+    <col min="5" max="5" width="10.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="8">
-        <f>SUM(E7:E33)</f>
-        <v>45.279999999999994</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+        <f>SUM(E7:E38)</f>
+        <v>81.430000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -577,7 +658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -601,251 +682,406 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5">
-        <v>22.61</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" ref="E8:E33" si="0">C8*D8</f>
-        <v>22.61</v>
+        <v>35</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5">
+        <v>22.61</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" ref="E9:E38" si="0">C9*D9</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A9" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C10" s="5">
         <v>1.59</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>6</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E10" s="5">
         <f t="shared" si="0"/>
         <v>9.5400000000000009</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>17</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C11" s="5">
         <v>4.32</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5">
-        <f t="shared" si="0"/>
-        <v>4.32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="5">
-        <v>1.1599999999999999</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="0"/>
+        <v>4.32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F11" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F12" t="s">
         <v>25</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="E12" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1.32</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+        <v>3.51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="5">
+        <v>3.6</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+        <v>7.2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.32</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+        <v>1.6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.32</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
       <c r="E17" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+        <v>3.2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.33</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
       <c r="E18" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A19" s="2" t="s">
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A20" s="9">
+      <c r="E24" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
         <v>559350210</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C25" s="5">
         <v>0.48</v>
       </c>
-      <c r="D20">
+      <c r="D25">
         <v>5</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E25" s="5">
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F25" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="E21" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="E22" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="E23" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="E24" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="E25" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E26" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E27" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E28" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E29" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E30" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E31" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E32" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -860,16 +1096,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3555E04D-A003-41C2-8A9A-B1D0F27D6347}">
   <dimension ref="A4:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.64453125" customWidth="1"/>
+    <col min="1" max="1" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -877,7 +1113,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
completed schematic of esc
</commit_message>
<xml_diff>
--- a/eagle/bom.xlsx
+++ b/eagle/bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\prj\qc\eagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5A3C06-BED3-479D-8B8A-B6C28AB462C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11846192-0401-4F7E-B7AE-8EB65766734D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7FFDE957-DDFA-40C3-B4B1-FC23B9487616}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>MFG NUM</t>
   </si>
@@ -219,6 +219,48 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/EEE-1VA100WR/PCE3948CT-ND/766324</t>
+  </si>
+  <si>
+    <t>molex</t>
+  </si>
+  <si>
+    <t>WM12296-ND</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole, Right Angle 2 position 0.079" (2.00mm)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=559350230</t>
+  </si>
+  <si>
+    <t>WM1375-ND</t>
+  </si>
+  <si>
+    <t>Connector Header Surface Mount, Right Angle 2 position 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=015913024</t>
+  </si>
+  <si>
+    <t>23-0015388020-ND</t>
+  </si>
+  <si>
+    <t>2 Position CIC, FFC Connector Receptacle 0.100" (2.54mm) Free Hanging (In-Line)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/molex/0015388020/23-0015388020-ND/505815</t>
+  </si>
+  <si>
+    <t>478-3451-1-ND</t>
+  </si>
+  <si>
+    <t>TCJA106M016R0200</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/avx-corporation/TCJA106M016R0200/478-3451-1-ND/998456</t>
+  </si>
+  <si>
+    <t>10µF Molded Tantalum Polymer Capacitor 16V 1206 (3216 Metric) 200mOhm @ 100kHz</t>
   </si>
 </sst>
 </file>
@@ -228,7 +270,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +293,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -269,11 +319,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -295,9 +346,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -610,11 +665,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA596EF-40FD-4069-B258-04479C4B0B2E}">
-  <dimension ref="A2:G38"/>
+  <dimension ref="A2:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,8 +686,8 @@
         <v>14</v>
       </c>
       <c r="G2" s="8">
-        <f>SUM(E7:E38)</f>
-        <v>81.430000000000007</v>
+        <f>SUM(E7:E41)</f>
+        <v>100.03999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -719,7 +774,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" ref="E9:E38" si="0">C9*D9</f>
+        <f t="shared" ref="E9:E41" si="0">C9*D9</f>
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -946,9 +1001,27 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
       <c r="E19" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.2200000000000006</v>
+      </c>
+      <c r="F19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -964,84 +1037,143 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
       <c r="E22" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
       <c r="E23" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="9"/>
+      <c r="E24" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="E25" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="E26" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="E27" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
         <v>559350210</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C28" s="5">
         <v>0.48</v>
       </c>
-      <c r="D25">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>559350230</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <f>C29*D29</f>
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>15913024</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1.91</v>
+      </c>
+      <c r="D30">
         <v>5</v>
       </c>
-      <c r="E25" s="5">
-        <f t="shared" si="0"/>
-        <v>2.4</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E26" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E28" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E29" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E30" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C30*D30</f>
+        <v>9.5499999999999989</v>
+      </c>
+      <c r="F30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>15388020</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="5">
+        <v>0.624</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
       <c r="E31" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C31*D31</f>
+        <v>6.24</v>
+      </c>
+      <c r="F31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1082,6 +1214,24 @@
     </row>
     <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1097,7 +1247,7 @@
   <dimension ref="A4:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,6 +1263,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>151360202</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
@@ -1122,6 +1280,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" display="https://www.molex.com/molex/search/partSearch?query=151360202&amp;pQuery=" xr:uid="{9F85A77B-BE9C-4A2F-99D2-0C4593198526}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>